<commit_message>
add class 3 material
</commit_message>
<xml_diff>
--- a/Clase 2/data/caso_restaurante_sabor_cauca.xlsx
+++ b/Clase 2/data/caso_restaurante_sabor_cauca.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabod\OneDrive\Documentos\UniMayor\Módulo 1\Clase 2\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{471A5023-0BF1-4453-9D12-17F995635C3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="40920" yWindow="-120" windowWidth="15600" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -49,11 +55,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,13 +123,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -161,7 +175,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -195,6 +209,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -229,9 +244,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -404,14 +420,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -431,7 +449,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
         <v>45658</v>
       </c>
@@ -451,7 +469,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
         <v>45658</v>
       </c>
@@ -471,7 +489,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="2">
         <v>45658</v>
       </c>
@@ -491,7 +509,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>45658</v>
       </c>
@@ -511,7 +529,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <v>45659</v>
       </c>
@@ -531,7 +549,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <v>45659</v>
       </c>
@@ -551,7 +569,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
         <v>45659</v>
       </c>
@@ -571,7 +589,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
         <v>45659</v>
       </c>
@@ -588,10 +606,10 @@
         <v>9246</v>
       </c>
       <c r="F9">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
         <v>45660</v>
       </c>
@@ -611,7 +629,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
         <v>45660</v>
       </c>
@@ -631,7 +649,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="2">
         <v>45660</v>
       </c>
@@ -651,7 +669,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="2">
         <v>45660</v>
       </c>
@@ -671,7 +689,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="2">
         <v>45661</v>
       </c>
@@ -691,7 +709,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="2">
         <v>45661</v>
       </c>
@@ -711,7 +729,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="2">
         <v>45661</v>
       </c>
@@ -731,7 +749,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="2">
         <v>45661</v>
       </c>
@@ -751,7 +769,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="2">
         <v>45662</v>
       </c>
@@ -771,7 +789,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="2">
         <v>45662</v>
       </c>
@@ -791,7 +809,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="2">
         <v>45662</v>
       </c>
@@ -811,7 +829,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="2">
         <v>45662</v>
       </c>
@@ -831,7 +849,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="2">
         <v>45663</v>
       </c>
@@ -851,7 +869,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="2">
         <v>45663</v>
       </c>
@@ -871,7 +889,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="2">
         <v>45663</v>
       </c>
@@ -891,7 +909,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="2">
         <v>45663</v>
       </c>
@@ -911,7 +929,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="2">
         <v>45664</v>
       </c>
@@ -931,7 +949,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="2">
         <v>45664</v>
       </c>
@@ -951,7 +969,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="2">
         <v>45664</v>
       </c>
@@ -971,7 +989,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="2">
         <v>45664</v>
       </c>
@@ -991,7 +1009,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="2">
         <v>45665</v>
       </c>
@@ -1011,7 +1029,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="2">
         <v>45665</v>
       </c>
@@ -1031,7 +1049,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="2">
         <v>45665</v>
       </c>
@@ -1051,7 +1069,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="2">
         <v>45665</v>
       </c>
@@ -1071,7 +1089,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="2">
         <v>45666</v>
       </c>
@@ -1091,7 +1109,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="2">
         <v>45666</v>
       </c>
@@ -1111,7 +1129,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="2">
         <v>45666</v>
       </c>
@@ -1131,7 +1149,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="2">
         <v>45666</v>
       </c>
@@ -1151,7 +1169,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="2">
         <v>45667</v>
       </c>
@@ -1171,7 +1189,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="2">
         <v>45667</v>
       </c>
@@ -1191,7 +1209,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="2">
         <v>45667</v>
       </c>
@@ -1211,7 +1229,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="2">
         <v>45667</v>
       </c>
@@ -1231,7 +1249,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="2">
         <v>45668</v>
       </c>
@@ -1251,7 +1269,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="2">
         <v>45668</v>
       </c>
@@ -1271,7 +1289,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="2">
         <v>45668</v>
       </c>
@@ -1291,7 +1309,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="2">
         <v>45668</v>
       </c>
@@ -1311,7 +1329,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" s="2">
         <v>45669</v>
       </c>
@@ -1331,7 +1349,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="2">
         <v>45669</v>
       </c>
@@ -1351,7 +1369,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" s="2">
         <v>45669</v>
       </c>
@@ -1371,7 +1389,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="2">
         <v>45669</v>
       </c>
@@ -1391,7 +1409,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="2">
         <v>45670</v>
       </c>
@@ -1411,7 +1429,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="2">
         <v>45670</v>
       </c>
@@ -1431,7 +1449,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="2">
         <v>45670</v>
       </c>
@@ -1451,7 +1469,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" s="2">
         <v>45670</v>
       </c>
@@ -1471,7 +1489,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" s="2">
         <v>45671</v>
       </c>
@@ -1491,7 +1509,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" s="2">
         <v>45671</v>
       </c>
@@ -1511,7 +1529,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" s="2">
         <v>45671</v>
       </c>
@@ -1531,7 +1549,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57" s="2">
         <v>45671</v>
       </c>
@@ -1551,7 +1569,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" s="2">
         <v>45672</v>
       </c>
@@ -1571,7 +1589,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" s="2">
         <v>45672</v>
       </c>
@@ -1591,7 +1609,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" s="2">
         <v>45672</v>
       </c>
@@ -1611,7 +1629,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" s="2">
         <v>45672</v>
       </c>
@@ -1631,7 +1649,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62" s="2">
         <v>45673</v>
       </c>
@@ -1651,7 +1669,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63" s="2">
         <v>45673</v>
       </c>
@@ -1671,7 +1689,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" s="2">
         <v>45673</v>
       </c>
@@ -1691,7 +1709,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" s="2">
         <v>45673</v>
       </c>
@@ -1711,7 +1729,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" s="2">
         <v>45674</v>
       </c>
@@ -1731,7 +1749,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" s="2">
         <v>45674</v>
       </c>
@@ -1751,7 +1769,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68" s="2">
         <v>45674</v>
       </c>
@@ -1771,7 +1789,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69" s="2">
         <v>45674</v>
       </c>
@@ -1791,7 +1809,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" s="2">
         <v>45675</v>
       </c>
@@ -1811,7 +1829,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A71" s="2">
         <v>45675</v>
       </c>
@@ -1831,7 +1849,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A72" s="2">
         <v>45675</v>
       </c>
@@ -1851,7 +1869,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A73" s="2">
         <v>45675</v>
       </c>
@@ -1871,7 +1889,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A74" s="2">
         <v>45676</v>
       </c>
@@ -1891,7 +1909,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A75" s="2">
         <v>45676</v>
       </c>
@@ -1911,7 +1929,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A76" s="2">
         <v>45676</v>
       </c>
@@ -1931,7 +1949,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A77" s="2">
         <v>45676</v>
       </c>
@@ -1951,7 +1969,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A78" s="2">
         <v>45677</v>
       </c>
@@ -1971,7 +1989,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A79" s="2">
         <v>45677</v>
       </c>
@@ -1991,7 +2009,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A80" s="2">
         <v>45677</v>
       </c>
@@ -2011,7 +2029,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A81" s="2">
         <v>45677</v>
       </c>
@@ -2031,7 +2049,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A82" s="2">
         <v>45678</v>
       </c>
@@ -2051,7 +2069,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A83" s="2">
         <v>45678</v>
       </c>
@@ -2071,7 +2089,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A84" s="2">
         <v>45678</v>
       </c>
@@ -2091,7 +2109,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A85" s="2">
         <v>45678</v>
       </c>
@@ -2111,7 +2129,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A86" s="2">
         <v>45679</v>
       </c>
@@ -2131,7 +2149,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A87" s="2">
         <v>45679</v>
       </c>
@@ -2151,7 +2169,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A88" s="2">
         <v>45679</v>
       </c>
@@ -2171,7 +2189,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A89" s="2">
         <v>45679</v>
       </c>
@@ -2191,7 +2209,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A90" s="2">
         <v>45680</v>
       </c>
@@ -2211,7 +2229,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A91" s="2">
         <v>45680</v>
       </c>
@@ -2231,7 +2249,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A92" s="2">
         <v>45680</v>
       </c>
@@ -2251,7 +2269,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A93" s="2">
         <v>45680</v>
       </c>
@@ -2271,7 +2289,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A94" s="2">
         <v>45681</v>
       </c>
@@ -2291,7 +2309,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A95" s="2">
         <v>45681</v>
       </c>
@@ -2311,7 +2329,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A96" s="2">
         <v>45681</v>
       </c>
@@ -2331,7 +2349,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A97" s="2">
         <v>45681</v>
       </c>
@@ -2351,7 +2369,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A98" s="2">
         <v>45682</v>
       </c>
@@ -2371,7 +2389,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A99" s="2">
         <v>45682</v>
       </c>
@@ -2391,7 +2409,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A100" s="2">
         <v>45682</v>
       </c>
@@ -2411,7 +2429,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="101" spans="1:6">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A101" s="2">
         <v>45682</v>
       </c>
@@ -2431,7 +2449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:6">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A102" s="2">
         <v>45683</v>
       </c>
@@ -2451,7 +2469,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="103" spans="1:6">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A103" s="2">
         <v>45683</v>
       </c>
@@ -2471,7 +2489,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="104" spans="1:6">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A104" s="2">
         <v>45683</v>
       </c>
@@ -2491,7 +2509,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="105" spans="1:6">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A105" s="2">
         <v>45683</v>
       </c>
@@ -2511,7 +2529,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="106" spans="1:6">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A106" s="2">
         <v>45684</v>
       </c>
@@ -2531,7 +2549,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="107" spans="1:6">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A107" s="2">
         <v>45684</v>
       </c>
@@ -2551,7 +2569,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A108" s="2">
         <v>45684</v>
       </c>
@@ -2571,7 +2589,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="109" spans="1:6">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A109" s="2">
         <v>45684</v>
       </c>
@@ -2591,7 +2609,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="110" spans="1:6">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A110" s="2">
         <v>45685</v>
       </c>
@@ -2611,7 +2629,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="111" spans="1:6">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A111" s="2">
         <v>45685</v>
       </c>
@@ -2631,7 +2649,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="112" spans="1:6">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A112" s="2">
         <v>45685</v>
       </c>
@@ -2651,7 +2669,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="113" spans="1:6">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A113" s="2">
         <v>45685</v>
       </c>
@@ -2671,7 +2689,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="114" spans="1:6">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A114" s="2">
         <v>45686</v>
       </c>
@@ -2691,7 +2709,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="115" spans="1:6">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A115" s="2">
         <v>45686</v>
       </c>
@@ -2711,7 +2729,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="116" spans="1:6">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A116" s="2">
         <v>45686</v>
       </c>
@@ -2731,7 +2749,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="117" spans="1:6">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A117" s="2">
         <v>45686</v>
       </c>
@@ -2751,7 +2769,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="118" spans="1:6">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A118" s="2">
         <v>45687</v>
       </c>
@@ -2771,7 +2789,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="119" spans="1:6">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A119" s="2">
         <v>45687</v>
       </c>
@@ -2791,7 +2809,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="1:6">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A120" s="2">
         <v>45687</v>
       </c>
@@ -2811,7 +2829,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="121" spans="1:6">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A121" s="2">
         <v>45687</v>
       </c>

</xml_diff>